<commit_message>
Fix a data problem. Find a data problem.
</commit_message>
<xml_diff>
--- a/data/xls/enrollment-1994.xlsx
+++ b/data/xls/enrollment-1994.xlsx
@@ -11153,8 +11153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1789"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1737" workbookViewId="0">
-      <selection activeCell="A1790" sqref="A1790"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>